<commit_message>
Calcula novas variáveis e exporta os resultados
</commit_message>
<xml_diff>
--- a/data/tbl_wilcox.xlsx
+++ b/data/tbl_wilcox.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -501,14 +501,14 @@
     </row>
     <row r="7">
       <c r="A7">
-        <v>537</v>
+        <v>827</v>
       </c>
       <c r="B7">
-        <v>0.3256304515919216</v>
+        <v>0.04369004672153537</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Wilcoxon rank sum exact test</t>
+          <t>Wilcoxon rank sum test with continuity correction</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -518,20 +518,20 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>p1 ~ media_v2</t>
+          <t>i1 ~ media_v1</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>555</v>
+        <v>625</v>
       </c>
       <c r="B8">
-        <v>0.4373968125481567</v>
+        <v>0.8029677201588449</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Wilcoxon rank sum exact test</t>
+          <t>Wilcoxon rank sum test with continuity correction</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -541,16 +541,16 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>p2 ~ media_v2</t>
+          <t>i2 ~ media_v1</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>733</v>
+        <v>537</v>
       </c>
       <c r="B9">
-        <v>0.2122279251510636</v>
+        <v>0.3256304515919216</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -564,16 +564,16 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>r1 ~ media_v2</t>
+          <t>p1 ~ media_v2</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10">
-        <v>740</v>
+        <v>555</v>
       </c>
       <c r="B10">
-        <v>0.1841164168323889</v>
+        <v>0.4373968125481567</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
@@ -587,16 +587,16 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>r2 ~ media_v2</t>
+          <t>p2 ~ media_v2</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11">
-        <v>742</v>
+        <v>733</v>
       </c>
       <c r="B11">
-        <v>0.1766083506160379</v>
+        <v>0.2122279251510636</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
@@ -610,20 +610,20 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>r3 ~ media_v2</t>
+          <t>r1 ~ media_v2</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12">
-        <v>393</v>
+        <v>740</v>
       </c>
       <c r="B12">
-        <v>0.1117474076557653</v>
+        <v>0.1841164168323889</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Wilcoxon rank sum test with continuity correction</t>
+          <t>Wilcoxon rank sum exact test</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -633,20 +633,20 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>p1 ~ media_v3</t>
+          <t>r2 ~ media_v2</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13">
-        <v>393</v>
+        <v>742</v>
       </c>
       <c r="B13">
-        <v>0.1117474076557653</v>
+        <v>0.1766083506160379</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Wilcoxon rank sum test with continuity correction</t>
+          <t>Wilcoxon rank sum exact test</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -656,16 +656,16 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>p2 ~ media_v3</t>
+          <t>r3 ~ media_v2</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14">
-        <v>668</v>
+        <v>743</v>
       </c>
       <c r="B14">
-        <v>0.06368126808427531</v>
+        <v>0.1717789922490576</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
@@ -679,16 +679,16 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>r1 ~ media_v3</t>
+          <t>i1 ~ media_v2</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15">
-        <v>678</v>
+        <v>497</v>
       </c>
       <c r="B15">
-        <v>0.047689241617696</v>
+        <v>0.1453250431908469</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
@@ -702,30 +702,168 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>r2 ~ media_v3</t>
+          <t>i2 ~ media_v2</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16">
+        <v>393</v>
+      </c>
+      <c r="B16">
+        <v>0.1117474076557653</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Wilcoxon rank sum test with continuity correction</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>two.sided</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>p1 ~ media_v3</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17">
+        <v>393</v>
+      </c>
+      <c r="B17">
+        <v>0.1117474076557653</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Wilcoxon rank sum test with continuity correction</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>two.sided</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>p2 ~ media_v3</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18">
+        <v>668</v>
+      </c>
+      <c r="B18">
+        <v>0.06368126808427531</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Wilcoxon rank sum test with continuity correction</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>two.sided</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>r1 ~ media_v3</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19">
+        <v>678</v>
+      </c>
+      <c r="B19">
+        <v>0.047689241617696</v>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Wilcoxon rank sum test with continuity correction</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>two.sided</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>r2 ~ media_v3</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20">
         <v>699</v>
       </c>
-      <c r="B16">
+      <c r="B20">
         <v>0.02482313013329353</v>
       </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>Wilcoxon rank sum test with continuity correction</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>two.sided</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Wilcoxon rank sum test with continuity correction</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>two.sided</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
         <is>
           <t>r3 ~ media_v3</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21">
+        <v>615</v>
+      </c>
+      <c r="B21">
+        <v>0.2347280906791234</v>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Wilcoxon rank sum test with continuity correction</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>two.sided</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>i1 ~ media_v3</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22">
+        <v>499</v>
+      </c>
+      <c r="B22">
+        <v>0.7952970451071087</v>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Wilcoxon rank sum test with continuity correction</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>two.sided</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>i2 ~ media_v3</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Exporta alguns indicadores em formato docx
</commit_message>
<xml_diff>
--- a/data/tbl_wilcox.xlsx
+++ b/data/tbl_wilcox.xlsx
@@ -501,10 +501,10 @@
     </row>
     <row r="7">
       <c r="A7">
-        <v>827</v>
+        <v>828</v>
       </c>
       <c r="B7">
-        <v>0.04369004672153537</v>
+        <v>0.04252751383954506</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -662,10 +662,10 @@
     </row>
     <row r="14">
       <c r="A14">
-        <v>743</v>
+        <v>744</v>
       </c>
       <c r="B14">
-        <v>0.1717789922490576</v>
+        <v>0.1682054113418063</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
@@ -823,10 +823,10 @@
     </row>
     <row r="21">
       <c r="A21">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="B21">
-        <v>0.2347280906791234</v>
+        <v>0.229812642500469</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>

</xml_diff>